<commit_message>
Added New Case scenario
</commit_message>
<xml_diff>
--- a/src/main/java/com/primero/testdata/Primero.xlsx
+++ b/src/main/java/com/primero/testdata/Primero.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCases" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddNewCases" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,12 +21,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
   <si>
     <t xml:space="preserve">Meera Khan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cpimsid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssesmentDueDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_cpims_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panchalingam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-10-2024</t>
   </si>
 </sst>
 </file>
@@ -128,11 +156,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -153,4 +181,62 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Assign and resolve flag
</commit_message>
<xml_diff>
--- a/src/main/java/com/primero/testdata/Primero.xlsx
+++ b/src/main/java/com/primero/testdata/Primero.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCases" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="AddNewCases" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AssignFlag" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,12 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
   <si>
-    <t xml:space="preserve">Meera Khan</t>
+    <t xml:space="preserve">Janani Panchalingam</t>
   </si>
   <si>
     <t xml:space="preserve">Cpimsid</t>
@@ -54,6 +55,51 @@
   </si>
   <si>
     <t xml:space="preserve">10-10-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnflagReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Flag 12</t>
   </si>
 </sst>
 </file>
@@ -160,7 +206,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -190,11 +236,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -228,6 +274,176 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before report only added reportpage.java
</commit_message>
<xml_diff>
--- a/src/main/java/com/primero/testdata/Primero.xlsx
+++ b/src/main/java/com/primero/testdata/Primero.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,18 +18,18 @@
     <sheet name="RejectTransferCase" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="AssignCase" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="RemoteReferCase" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="AssignFlag" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="incident" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="edit_incident" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Setting_user" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="edit_user" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="edit_role" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="usergroup" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="edit_usergroup" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="Setting_AgencyAdd" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="edit_agency" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="forms_setting" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="forms_lookup" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="incident" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="edit_incident" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Setting_user" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="edit_user" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="edit_role" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="usergroup" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="edit_usergroup" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Setting_AgencyAdd" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="edit_agency" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="forms_setting" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="forms_lookup" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="AssignFlag" sheetId="22" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -41,12 +41,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
   <si>
-    <t xml:space="preserve">56da0e1</t>
+    <t xml:space="preserve">f2c56d4</t>
   </si>
   <si>
     <t xml:space="preserve">Cpimsid</t>
@@ -103,6 +103,9 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">aee68f7</t>
+  </si>
+  <si>
     <t xml:space="preserve">UNICEF</t>
   </si>
   <si>
@@ -115,16 +118,19 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">fc34ce0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comment For Approval</t>
   </si>
   <si>
-    <t xml:space="preserve">a79eecc</t>
+    <t xml:space="preserve">e0b2006</t>
   </si>
   <si>
     <t xml:space="preserve">Comment For Rejection</t>
   </si>
   <si>
-    <t xml:space="preserve">7b27380</t>
+    <t xml:space="preserve">b8ccfef</t>
   </si>
   <si>
     <t xml:space="preserve">Reason for Rejection</t>
@@ -133,7 +139,10 @@
     <t xml:space="preserve">Assignee</t>
   </si>
   <si>
-    <t xml:space="preserve">755866c</t>
+    <t xml:space="preserve">d0ca768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primero</t>
   </si>
   <si>
     <t xml:space="preserve">Ref</t>
@@ -142,16 +151,13 @@
     <t xml:space="preserve">Service</t>
   </si>
   <si>
-    <t xml:space="preserve">referagency</t>
-  </si>
-  <si>
     <t xml:space="preserve">location</t>
   </si>
   <si>
     <t xml:space="preserve">recipient</t>
   </si>
   <si>
-    <t xml:space="preserve">7bf7eed</t>
+    <t xml:space="preserve">fe64218</t>
   </si>
   <si>
     <t xml:space="preserve">CP</t>
@@ -160,184 +166,190 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search</t>
+    <t xml:space="preserve">vishu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">violence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeofday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">violencetype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sexual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nationalId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adec372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fullname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConfirmPwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">villa1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manz2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primero CP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testeropurv@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usecode_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test UserGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description is here please read carefully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test UG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descriptionghj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testAgency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FormGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestForm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Lookup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchtext</t>
   </si>
   <si>
     <t xml:space="preserve">reason</t>
   </si>
   <si>
-    <t xml:space="preserve">reasontounflag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bf5fa74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assign Flag Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">violence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeofday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">violencetype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nationality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nationalId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e9f3f3e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fullname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pwd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ConfirmPwd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">villa1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manz2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primero CP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testeropurv@test.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usecode_t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">villa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transfer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test UG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description is here please read carefully.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agency_Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A_123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FormGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestForm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Record Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Lookup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lookups</t>
+    <t xml:space="preserve">eason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assign Flag</t>
   </si>
 </sst>
 </file>
@@ -478,10 +490,10 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -489,7 +501,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -509,211 +521,162 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>37</v>
+      <c r="E2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>33</v>
@@ -733,7 +696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -744,64 +707,64 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="C2" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="D2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="H2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -820,6 +783,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -828,58 +831,61 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -888,6 +894,9 @@
       <c r="B2" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -905,63 +914,109 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>84</v>
+      </c>
       <c r="C1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>79</v>
@@ -969,63 +1024,11 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>89</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1045,11 +1048,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1101,60 +1104,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>90</v>
@@ -1174,7 +1137,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>95</v>
@@ -1194,7 +1157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1205,14 +1168,14 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,6 +1197,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1245,7 +1254,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -1394,7 +1403,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1425,10 +1434,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1445,14 +1454,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>19</v>
@@ -1477,25 +1486,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1516,26 +1525,26 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1556,11 +1565,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1581,19 +1590,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1618,22 +1627,22 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>